<commit_message>
meeting notes for first meeting
</commit_message>
<xml_diff>
--- a/Workframe.xlsx
+++ b/Workframe.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jenniferwu/Documents/kaggle-competition1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C92B9774-EB2B-A24F-BEEA-455F1AC3F05A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{414B8147-01FF-5E4B-A885-DCDC5BC789E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16420" activeTab="5" xr2:uid="{7543AB26-D562-434E-BAF0-9029E041A9BC}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16420" activeTab="2" xr2:uid="{7543AB26-D562-434E-BAF0-9029E041A9BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="67">
   <si>
     <t>Activities</t>
   </si>
@@ -202,6 +202,44 @@
   </si>
   <si>
     <t>Action Items</t>
+  </si>
+  <si>
+    <t>join key</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>1. We can use the lat &amp; long to predict if the spray is effective</t>
+  </si>
+  <si>
+    <t>3.  weather data is available for the whole time</t>
+  </si>
+  <si>
+    <t>4. look at weather data first --&gt; spray data --&gt; then the train</t>
+  </si>
+  <si>
+    <t>dttm</t>
+  </si>
+  <si>
+    <t>2. Spray data are incomplete (not for the entire time as the weather data)</t>
+  </si>
+  <si>
+    <t>1. Whether or not the virus is present for a given weather, time, seasonal activity, and location ?
+2. The distance between with trap and spray?
+3. How the weather &amp; humidity affects the virus presence?</t>
+  </si>
+  <si>
+    <t>learning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Cleaning = multiple records and non distinct data, need to change varchar into numeric </t>
+  </si>
+  <si>
+    <t>Need to look into the combined mosquito species (weather or not)</t>
+  </si>
+  <si>
+    <t>Most mosquito is found in August</t>
   </si>
 </sst>
 </file>
@@ -233,7 +271,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -293,11 +331,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -315,9 +366,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -333,6 +381,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -649,8 +707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90A4CC5D-A4FF-B94B-8A45-AE33DE0A5D2E}">
   <dimension ref="B2:H10"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -699,7 +757,7 @@
       </c>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:8" ht="170" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
         <v>5</v>
       </c>
@@ -708,7 +766,9 @@
       <c r="E4" s="2"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
-      <c r="H4" s="2"/>
+      <c r="H4" s="12" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
@@ -800,7 +860,7 @@
   <dimension ref="B2:D10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -808,7 +868,7 @@
     <col min="1" max="1" width="4.1640625" customWidth="1"/>
     <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="48.83203125" customWidth="1"/>
-    <col min="4" max="4" width="33.1640625" customWidth="1"/>
+    <col min="4" max="4" width="56.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
@@ -823,14 +883,16 @@
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="8">
+      <c r="B3" s="7">
         <v>43725</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="4"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="4" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B4" s="8">
+      <c r="B4" s="7">
         <v>43731</v>
       </c>
       <c r="C4" s="4"/>
@@ -873,19 +935,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3D26BE5-D38D-764A-B744-A1098FA04707}">
-  <dimension ref="B2:E17"/>
+  <dimension ref="B2:F26"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.1640625" customWidth="1"/>
     <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.33203125" customWidth="1"/>
+    <col min="6" max="6" width="79" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
         <v>21</v>
       </c>
@@ -898,126 +963,184 @@
       <c r="E2" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B3" s="10" t="s">
+      <c r="F2" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B3" s="9" t="s">
         <v>38</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="11"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="15"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B4" s="10"/>
       <c r="C4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="11"/>
+      <c r="D4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" s="16"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B5" s="10"/>
       <c r="C5" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="11"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="17"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B6" s="10"/>
       <c r="C6" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="11"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B7" s="10"/>
       <c r="C7" s="1" t="s">
         <v>28</v>
       </c>
       <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="11"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="16"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B8" s="10"/>
       <c r="C8" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="11"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="16"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="10"/>
       <c r="C9" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="11"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="16"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B10" s="10"/>
       <c r="C10" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="11"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="16"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="10"/>
       <c r="C11" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="11"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="16"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B12" s="10"/>
       <c r="C12" s="1" t="s">
         <v>34</v>
       </c>
       <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="11"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="16"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B13" s="10"/>
       <c r="C13" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B14" s="12"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="16"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="11"/>
       <c r="C14" s="1" t="s">
         <v>36</v>
       </c>
       <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="10" t="s">
+      <c r="E14" s="14"/>
+      <c r="F14" s="16"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B15" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B16" s="12"/>
+      <c r="D15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" s="16"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B16" s="11"/>
       <c r="C16" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17" s="7" t="s">
+      <c r="E16" s="14"/>
+      <c r="F16" s="16"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B17" s="2" t="s">
         <v>20</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1033,7 +1156,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{726F472E-D667-664A-8DE0-CF57AB99BC02}">
   <dimension ref="B2:E8"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1127,7 +1252,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{588FFED3-CA35-564E-B4B5-162654DBA586}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0"/>
+    <sheetView topLeftCell="A54" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>

</xml_diff>